<commit_message>
FETURE: Get Interest Rates
</commit_message>
<xml_diff>
--- a/src/interestRates/assets/report.xlsx
+++ b/src/interestRates/assets/report.xlsx
@@ -49,10 +49,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Was not able to save Interest Rates, 2022-09-05</t>
-  </si>
-  <si>
-    <t>2022-09-05 23:29:21</t>
+    <t>The interest Rates has a format error</t>
+  </si>
+  <si>
+    <t>2022-09-06 12:53:09</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
FEATURE: Interest Rates Loop
</commit_message>
<xml_diff>
--- a/src/interestRates/assets/report.xlsx
+++ b/src/interestRates/assets/report.xlsx
@@ -49,10 +49,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>The interest Rates has a format error</t>
-  </si>
-  <si>
-    <t>2022-09-06 12:53:09</t>
+    <t xml:space="preserve">Was not able to save Interest Rates, </t>
+  </si>
+  <si>
+    <t>2022-09-06 16:41:58</t>
   </si>
 </sst>
 </file>

</xml_diff>